<commit_message>
include pre-calculated yield_ug column
</commit_message>
<xml_diff>
--- a/data/raw/transcriptomics/20200320_transcriptomics_submission.xlsx
+++ b/data/raw/transcriptomics/20200320_transcriptomics_submission.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t xml:space="preserve">isolation_date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">ratio_260_280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yield_ug</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -101,11 +104,12 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,12 +125,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,10 +187,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,20 +209,20 @@
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -249,22 +243,24 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>39</v>
       </c>
       <c r="F2" s="1" t="n">
@@ -278,25 +274,29 @@
       </c>
       <c r="I2" s="1" t="n">
         <v>2.165</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <f aca="false">(F2*E2)/1000</f>
+        <v>1.882296</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>35.349</v>
       </c>
       <c r="G3" s="3" t="n">
@@ -305,27 +305,31 @@
       <c r="H3" s="4" t="n">
         <v>1.275</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>1.972</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <f aca="false">(F3*E3)/1000</f>
+        <v>1.378611</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>217.318</v>
       </c>
       <c r="G4" s="3" t="n">
@@ -334,269 +338,309 @@
       <c r="H4" s="4" t="n">
         <v>2.377</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>2.143</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <f aca="false">(F4*E4)/1000</f>
+        <v>8.475402</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>43880</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>37.851</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.9463</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>1.688</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>2.057</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <f aca="false">(F5*E5)/1000</f>
+        <v>2.233209</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>43880</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>456.805</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>11.4201</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>1.498</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>2.038</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <f aca="false">(F6*E6)/1000</f>
+        <v>17.815395</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>43880</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>250.171</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>6.2543</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>1.291</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>2.168</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <f aca="false">(F7*E7)/1000</f>
+        <v>9.756669</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>43881</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>79.931</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>1.9983</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>2.104</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>2.108</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <f aca="false">(F8*E8)/1000</f>
+        <v>3.117309</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>43881</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
+      <c r="B9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>437.871</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>10.9468</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1.862</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>2.125</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <f aca="false">(F9*E9)/1000</f>
+        <v>17.076969</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>43881</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>19</v>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>251.109</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>6.2777</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>2.195</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>2.152</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <f aca="false">(F10*E10)/1000</f>
+        <v>9.793251</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>20</v>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>51.791</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>1.2948</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.159</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="1" t="n">
         <v>2.083</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">(F11*E11)/1000</f>
+        <v>2.019849</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>68.993</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>1.7248</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>0.918</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <v>2.112</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <f aca="false">(F12*E12)/1000</f>
+        <v>2.690727</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>66.307</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>1.6577</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>0.34</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="1" t="n">
         <v>2.116</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <f aca="false">(F13*E13)/1000</f>
+        <v>2.585973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>